<commit_message>
Combining TicTacToe results and adding titles/labels to all graphs
</commit_message>
<xml_diff>
--- a/results/ChungToiEpsilonResults_1MillionGames.xlsx
+++ b/results/ChungToiEpsilonResults_1MillionGames.xlsx
@@ -581,6 +581,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Number of Games (out of 1 million played</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t>) vs Epsilon</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -2490,40 +2514,94 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="7831936"/>
-        <c:axId val="7834240"/>
+        <c:axId val="175309184"/>
+        <c:axId val="175310720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="7831936"/>
+        <c:axId val="175309184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Epsilon</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.4694610786011299"/>
+              <c:y val="0.91682117054955758"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="7834240"/>
+        <c:crossAx val="175310720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickLblSkip val="10"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7834240"/>
+        <c:axId val="175310720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t># of Games</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.4446227929373997E-2"/>
+              <c:y val="0.40260464864572343"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="7831936"/>
+        <c:crossAx val="175309184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2550,15 +2628,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>